<commit_message>
Sua loi mot so tinh nang
</commit_message>
<xml_diff>
--- a/DLMauGV.xlsx
+++ b/DLMauGV.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>CMND</t>
   </si>
@@ -33,13 +33,7 @@
     <t>Lê Quang Vinh</t>
   </si>
   <si>
-    <t>21/10/199</t>
-  </si>
-  <si>
-    <t>ABC</t>
-  </si>
-  <si>
-    <t>11/11/111</t>
+    <t>Trương Văn Khôi</t>
   </si>
 </sst>
 </file>
@@ -75,8 +69,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -360,13 +355,14 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.77734375" customWidth="1"/>
+    <col min="3" max="3" width="12.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -382,24 +378,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>5</v>
+        <v>987654321</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
+      <c r="C2" s="1">
+        <v>36454</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>123456783</v>
+        <v>987654322</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="C3" s="1">
+        <v>36475</v>
       </c>
     </row>
   </sheetData>

</xml_diff>